<commit_message>
add some result spreadsheets
</commit_message>
<xml_diff>
--- a/results/sampled_results/faultproneness_sampled_sumary.xlsx
+++ b/results/sampled_results/faultproneness_sampled_sumary.xlsx
@@ -367,6 +367,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -388,6 +389,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -460,8 +462,8 @@
   </sheetPr>
   <dimension ref="A1:C109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B109" activeCellId="0" sqref="B109"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C109" activeCellId="0" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -906,10 +908,10 @@
         <v>41</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>255</v>
+        <v>210</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>2279</v>
+        <v>1858</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1666,11 +1668,11 @@
       </c>
       <c r="B109" s="1" t="n">
         <f aca="false">SUM(B2:B108)</f>
-        <v>309</v>
+        <v>264</v>
       </c>
       <c r="C109" s="1" t="n">
         <f aca="false">SUM(C2:C108)</f>
-        <v>2693</v>
+        <v>2272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>